<commit_message>
v2.00 - All tests pass, ready to refactor for Switch Statement Smell
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -2194,6 +2194,27 @@
       </c>
     </row>
     <row r="13" spans="1:3150">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>42</v>
+      </c>
+      <c r="D13" t="n">
+        <v>666</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>180</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
       <c r="AX13" t="s">
         <v>20</v>
       </c>
@@ -2301,6 +2322,27 @@
       </c>
     </row>
     <row r="14" spans="1:3150">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>42</v>
+      </c>
+      <c r="D14" t="n">
+        <v>666</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>180</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
       <c r="BE14" t="s">
         <v>22</v>
       </c>
@@ -2408,6 +2450,27 @@
       </c>
     </row>
     <row r="15" spans="1:3150">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>42</v>
+      </c>
+      <c r="D15" t="n">
+        <v>666</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>180</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
       <c r="BL15" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
v2.01 - Created fix for Duplicate Code smell, implemented 1 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -2578,6 +2578,27 @@
       </c>
     </row>
     <row r="16" spans="1:3150">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>42</v>
+      </c>
+      <c r="D16" t="n">
+        <v>666</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>180</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
       <c r="BS16" t="s">
         <v>26</v>
       </c>
@@ -2685,6 +2706,27 @@
       </c>
     </row>
     <row r="17" spans="1:3150">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>42</v>
+      </c>
+      <c r="D17" t="n">
+        <v>666</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>180</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
       <c r="BZ17" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
v2.02 - Created fix for Duplicate Code smell, implemented 2 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -2834,6 +2834,27 @@
       </c>
     </row>
     <row r="18" spans="1:3150">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>42</v>
+      </c>
+      <c r="D18" t="n">
+        <v>666</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>180</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
       <c r="CG18" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
v2.03 - Modified fix for Duplicate Code smell, implemented 3 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -2962,6 +2962,27 @@
       </c>
     </row>
     <row r="19" spans="1:3150">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>42</v>
+      </c>
+      <c r="D19" t="n">
+        <v>666</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>180</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
       <c r="CN19" t="s">
         <v>31</v>
       </c>
@@ -3069,6 +3090,27 @@
       </c>
     </row>
     <row r="20" spans="1:3150">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>42</v>
+      </c>
+      <c r="D20" t="n">
+        <v>666</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>180</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
       <c r="CU20" t="s">
         <v>33</v>
       </c>
@@ -3176,6 +3218,27 @@
       </c>
     </row>
     <row r="21" spans="1:3150">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42</v>
+      </c>
+      <c r="D21" t="n">
+        <v>666</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>180</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
       <c r="DB21" t="s">
         <v>35</v>
       </c>
@@ -3283,6 +3346,27 @@
       </c>
     </row>
     <row r="22" spans="1:3150">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>42</v>
+      </c>
+      <c r="D22" t="n">
+        <v>666</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>180</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
       <c r="DI22" t="s">
         <v>37</v>
       </c>
@@ -3390,6 +3474,27 @@
       </c>
     </row>
     <row r="23" spans="1:3150">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>42</v>
+      </c>
+      <c r="D23" t="n">
+        <v>666</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>180</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
       <c r="DP23" t="s">
         <v>39</v>
       </c>
@@ -3497,6 +3602,27 @@
       </c>
     </row>
     <row r="24" spans="1:3150">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>42</v>
+      </c>
+      <c r="D24" t="n">
+        <v>666</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>180</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
       <c r="DW24" t="s">
         <v>41</v>
       </c>
@@ -3604,6 +3730,27 @@
       </c>
     </row>
     <row r="25" spans="1:3150">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>42</v>
+      </c>
+      <c r="D25" t="n">
+        <v>666</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>180</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
       <c r="ED25" t="s">
         <v>43</v>
       </c>
@@ -3711,6 +3858,27 @@
       </c>
     </row>
     <row r="26" spans="1:3150">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>42</v>
+      </c>
+      <c r="D26" t="n">
+        <v>666</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="n">
+        <v>180</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
       <c r="EK26" t="s">
         <v>45</v>
       </c>
@@ -3818,6 +3986,27 @@
       </c>
     </row>
     <row r="27" spans="1:3150">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>42</v>
+      </c>
+      <c r="D27" t="n">
+        <v>666</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>180</v>
+      </c>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
       <c r="ER27" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
v2.04 - Implemented fix for Duplicate Code smell, implemented 4 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4114,6 +4114,27 @@
       </c>
     </row>
     <row r="28" spans="1:3150">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>42</v>
+      </c>
+      <c r="D28" t="n">
+        <v>666</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="n">
+        <v>180</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
       <c r="EY28" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
v2.05 - Implemented fix for Duplicate Code smell, implemented 5 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4242,6 +4242,27 @@
       </c>
     </row>
     <row r="29" spans="1:3150">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>42</v>
+      </c>
+      <c r="D29" t="n">
+        <v>666</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="n">
+        <v>180</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
       <c r="FF29" t="s">
         <v>54</v>
       </c>
@@ -4349,6 +4370,27 @@
       </c>
     </row>
     <row r="30" spans="1:3150">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>42</v>
+      </c>
+      <c r="D30" t="n">
+        <v>666</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="n">
+        <v>180</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
       <c r="FM30" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
v2.05.5 - Modified an implementation of fix for Duplicate Code smell, implemented 5 of 12.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4498,6 +4498,27 @@
       </c>
     </row>
     <row r="31" spans="1:3150">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>42</v>
+      </c>
+      <c r="D31" t="n">
+        <v>666</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="n">
+        <v>180</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
       <c r="FT31" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
v2.06 - Implemented fix for Duplicate Code smell, implemented 6 of 11. *Previous numbering is incorrect, only 11 methods to change.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4626,6 +4626,27 @@
       </c>
     </row>
     <row r="32" spans="1:3150">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>42</v>
+      </c>
+      <c r="D32" t="n">
+        <v>666</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="n">
+        <v>180</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
       <c r="GA32" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
v2.06.5 - Implemented fix for Duplicate Code smell, implemented 6 of 9. *Previous numbering is incorrect, only 9 methods to change as save/load pickle does not use flags, but still requires argument.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4754,6 +4754,27 @@
       </c>
     </row>
     <row r="33" spans="1:3150">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>42</v>
+      </c>
+      <c r="D33" t="n">
+        <v>666</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>180</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
       <c r="GH33" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
v2.07 - Implemented fix for Duplicate Code smell, implemented 7 of 9.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -4882,6 +4882,27 @@
       </c>
     </row>
     <row r="34" spans="1:3150">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>42</v>
+      </c>
+      <c r="D34" t="n">
+        <v>666</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="n">
+        <v>180</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
       <c r="GO34" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
v2.08 - Implemented fix for Duplicate Code smell, implemented 8 of 9.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5010,6 +5010,27 @@
       </c>
     </row>
     <row r="35" spans="1:3150">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>42</v>
+      </c>
+      <c r="D35" t="n">
+        <v>666</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="n">
+        <v>180</v>
+      </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
       <c r="GV35" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
v2.09 - Implemented fix for Duplicate Code smell, implemented 9 of 9. All tests passed. 99% branch coverage (100 for changed code)
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5138,6 +5138,27 @@
       </c>
     </row>
     <row r="36" spans="1:3150">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>42</v>
+      </c>
+      <c r="D36" t="n">
+        <v>666</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="n">
+        <v>180</v>
+      </c>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
       <c r="HC36" t="s">
         <v>69</v>
       </c>
@@ -5245,6 +5266,27 @@
       </c>
     </row>
     <row r="37" spans="1:3150">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>42</v>
+      </c>
+      <c r="D37" t="n">
+        <v>666</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>180</v>
+      </c>
+      <c r="G37" t="s">
+        <v>16</v>
+      </c>
       <c r="HJ37" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
v3.00 - Passed all tests, 99% branch coverage (100 for target code). Ready for Long Method fix.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5394,6 +5394,27 @@
       </c>
     </row>
     <row r="38" spans="1:3150">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>42</v>
+      </c>
+      <c r="D38" t="n">
+        <v>666</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="n">
+        <v>180</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
       <c r="HQ38" t="s">
         <v>73</v>
       </c>
@@ -5501,6 +5522,27 @@
       </c>
     </row>
     <row r="39" spans="1:3150">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>42</v>
+      </c>
+      <c r="D39" t="n">
+        <v>666</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="n">
+        <v>180</v>
+      </c>
+      <c r="G39" t="s">
+        <v>16</v>
+      </c>
       <c r="HX39" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
v3.01 - First modification of Long Method fix. Implemented 1 of 2
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5650,6 +5650,27 @@
       </c>
     </row>
     <row r="40" spans="1:3150">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>42</v>
+      </c>
+      <c r="D40" t="n">
+        <v>666</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" t="n">
+        <v>180</v>
+      </c>
+      <c r="G40" t="s">
+        <v>16</v>
+      </c>
       <c r="IE40" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
v3.01.2 - First modification of Long Method fix. Implemented 2 of 2
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5778,6 +5778,27 @@
       </c>
     </row>
     <row r="41" spans="1:3150">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>42</v>
+      </c>
+      <c r="D41" t="n">
+        <v>666</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="n">
+        <v>180</v>
+      </c>
+      <c r="G41" t="s">
+        <v>16</v>
+      </c>
       <c r="IL41" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
v3.02 - Second modification of Long Method fix. Implemented 1 of 1
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -5906,6 +5906,27 @@
       </c>
     </row>
     <row r="42" spans="1:3150">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>42</v>
+      </c>
+      <c r="D42" t="n">
+        <v>666</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" t="n">
+        <v>180</v>
+      </c>
+      <c r="G42" t="s">
+        <v>16</v>
+      </c>
       <c r="IS42" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
v3.03 - Third modification of Long Method fix. Implemented 1 of 1
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6034,6 +6034,27 @@
       </c>
     </row>
     <row r="43" spans="1:3150">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>42</v>
+      </c>
+      <c r="D43" t="n">
+        <v>666</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>180</v>
+      </c>
+      <c r="G43" t="s">
+        <v>16</v>
+      </c>
       <c r="IZ43" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
v3.04.1 - Fourth modification of Long Method fix. Implemented 1 of 2
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6162,6 +6162,27 @@
       </c>
     </row>
     <row r="44" spans="1:3150">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>42</v>
+      </c>
+      <c r="D44" t="n">
+        <v>666</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="n">
+        <v>180</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
+      </c>
       <c r="JG44" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
v3.04.2 - Fourth modification of Long Method fix. Implemented 2 of 2
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6290,6 +6290,27 @@
       </c>
     </row>
     <row r="45" spans="1:3150">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>42</v>
+      </c>
+      <c r="D45" t="n">
+        <v>666</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="n">
+        <v>180</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
+      </c>
       <c r="JN45" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
v4.00 - Passed all tests. 99% branch coverage (missing end of elif statement, will be fixed). Ready for refactoring Switch Statement
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6418,6 +6418,27 @@
       </c>
     </row>
     <row r="46" spans="1:3150">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="n">
+        <v>42</v>
+      </c>
+      <c r="D46" t="n">
+        <v>666</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>180</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
       <c r="JU46" t="s">
         <v>89</v>
       </c>
@@ -6525,6 +6546,27 @@
       </c>
     </row>
     <row r="47" spans="1:3150">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="n">
+        <v>42</v>
+      </c>
+      <c r="D47" t="n">
+        <v>666</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="n">
+        <v>180</v>
+      </c>
+      <c r="G47" t="s">
+        <v>16</v>
+      </c>
       <c r="KB47" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
v4.02 - Switch Statement fixed. Implemented 1 of 1
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6674,6 +6674,27 @@
       </c>
     </row>
     <row r="48" spans="1:3150">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="n">
+        <v>42</v>
+      </c>
+      <c r="D48" t="n">
+        <v>666</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="n">
+        <v>180</v>
+      </c>
+      <c r="G48" t="s">
+        <v>16</v>
+      </c>
       <c r="KI48" t="s">
         <v>92</v>
       </c>
@@ -6781,6 +6802,27 @@
       </c>
     </row>
     <row r="49" spans="1:3150">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="n">
+        <v>42</v>
+      </c>
+      <c r="D49" t="n">
+        <v>666</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" t="n">
+        <v>180</v>
+      </c>
+      <c r="G49" t="s">
+        <v>16</v>
+      </c>
       <c r="KP49" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
v5.00 - All tests pass. 100% branch coverage. Ready to fix final Speculative Generality smell
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -6930,6 +6930,27 @@
       </c>
     </row>
     <row r="50" spans="1:3150">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>42</v>
+      </c>
+      <c r="D50" t="n">
+        <v>666</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" t="n">
+        <v>180</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
+      </c>
       <c r="KW50" t="s">
         <v>95</v>
       </c>
@@ -7037,6 +7058,27 @@
       </c>
     </row>
     <row r="51" spans="1:3150">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="n">
+        <v>42</v>
+      </c>
+      <c r="D51" t="n">
+        <v>666</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="n">
+        <v>180</v>
+      </c>
+      <c r="G51" t="s">
+        <v>16</v>
+      </c>
       <c r="LD51" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
v5.01.2 - First modification of Speculative Generality. Implements 2 of 2
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -7186,6 +7186,27 @@
       </c>
     </row>
     <row r="52" spans="1:3150">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>42</v>
+      </c>
+      <c r="D52" t="n">
+        <v>666</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" t="n">
+        <v>180</v>
+      </c>
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
       <c r="LK52" t="s">
         <v>97</v>
       </c>
@@ -7293,6 +7314,27 @@
       </c>
     </row>
     <row r="53" spans="1:3150">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="n">
+        <v>42</v>
+      </c>
+      <c r="D53" t="n">
+        <v>666</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="n">
+        <v>180</v>
+      </c>
+      <c r="G53" t="s">
+        <v>16</v>
+      </c>
       <c r="LR53" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
v5.02 - Second modification of Speculative Generality. Implements 1 of 1
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -7439,6 +7439,27 @@
       </c>
     </row>
     <row r="54" spans="1:3150">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>42</v>
+      </c>
+      <c r="D54" t="n">
+        <v>666</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>180</v>
+      </c>
+      <c r="G54" t="s">
+        <v>16</v>
+      </c>
       <c r="LY54" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
v6 - All tests passing. 100% branch coverage. 4 of 4 bad smells fixed.
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -7564,6 +7564,27 @@
       </c>
     </row>
     <row r="55" spans="1:3150">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="n">
+        <v>42</v>
+      </c>
+      <c r="D55" t="n">
+        <v>666</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>180</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
+      </c>
       <c r="MF55" t="s">
         <v>101</v>
       </c>

</xml_diff>